<commit_message>
Update Deposit, Product, dan Sales Report
</commit_message>
<xml_diff>
--- a/public/template/report/Template_Report_Product_Cost.xlsx
+++ b/public/template/report/Template_Report_Product_Cost.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0BCFF-7720-48C5-9C87-62FBEAF51AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516EDA69-9174-446F-9CAE-39FC51466828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report Growth" sheetId="1" r:id="rId1"/>
+    <sheet name="Report Cost" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>